<commit_message>
Commit and push July 18_1st
</commit_message>
<xml_diff>
--- a/New BDD Project/src/test/resources/Test Data/InputTestData.xlsx
+++ b/New BDD Project/src/test/resources/Test Data/InputTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jul16\New BDD Project\src\test\resources\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\July17th 2024\New BDD Project\src\test\resources\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAB74CC-E9D7-43E9-8C51-FAEA20C40A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11638A4E-1FBF-4778-A89D-70E90FF77B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>ac3nKr/qRTJJwHMCjJ2JuxVrEhlKlh6zpIcCUjvmch4hbynj6TblwdUufHaWef/C</t>
   </si>
@@ -92,6 +92,18 @@
   </si>
   <si>
     <t>https://www.google.com/account/about/?hl=en</t>
+  </si>
+  <si>
+    <t>rahulshettyacademy</t>
+  </si>
+  <si>
+    <t>8i9bJCh/kEhHUDzlbMIA8g==</t>
+  </si>
+  <si>
+    <t>https://rahulshettyacademy.com/loginpagePractise/</t>
+  </si>
+  <si>
+    <t>IND</t>
   </si>
 </sst>
 </file>
@@ -131,7 +143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -268,6 +280,47 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -275,7 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -309,6 +362,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -591,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,13 +719,13 @@
       <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" ht="259.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -679,9 +742,23 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G9" s="1"/>
-      <c r="H9"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G8" s="1"/>
+      <c r="H8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -690,8 +767,9 @@
     <hyperlink ref="B3" r:id="rId3" xr:uid="{5B824CF7-2024-4A32-9805-9CA5D8102D58}"/>
     <hyperlink ref="D3" r:id="rId4" xr:uid="{315AE5D7-87B5-4595-8ACD-29F81DF07AE6}"/>
     <hyperlink ref="H3" r:id="rId5" xr:uid="{AE380D6E-7373-4358-992A-5E58CE864723}"/>
+    <hyperlink ref="A4" r:id="rId6" xr:uid="{48EDFAD1-D101-4B77-9288-82C0A0E67CAF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit and keep - Aug 16th 2024
</commit_message>
<xml_diff>
--- a/New BDD Project/src/test/resources/Test Data/InputTestData.xlsx
+++ b/New BDD Project/src/test/resources/Test Data/InputTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\July17th 2024\New BDD Project\src\test\resources\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BDD-cucumber-Framework\New BDD Project\src\test\resources\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11638A4E-1FBF-4778-A89D-70E90FF77B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DD262B-CB6B-4923-BE31-CD89B7B40F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>ac3nKr/qRTJJwHMCjJ2JuxVrEhlKlh6zpIcCUjvmch4hbynj6TblwdUufHaWef/C</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>IND</t>
+  </si>
+  <si>
+    <t>https://qualitymatrix.greythr.com/</t>
+  </si>
+  <si>
+    <t>3ffSZVb8+St4jbFnc3BR9A==</t>
   </si>
 </sst>
 </file>
@@ -143,7 +149,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -215,7 +221,24 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -225,102 +248,48 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -333,9 +302,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -345,33 +311,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -654,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,94 +638,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H1" s="9"/>
     </row>
-    <row r="2" spans="1:8" ht="245.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:8" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" s="11"/>
     </row>
-    <row r="3" spans="1:8" ht="259.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:8" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>256</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="14">
+        <v>256</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="13"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>255</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>256</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -768,8 +768,9 @@
     <hyperlink ref="D3" r:id="rId4" xr:uid="{315AE5D7-87B5-4595-8ACD-29F81DF07AE6}"/>
     <hyperlink ref="H3" r:id="rId5" xr:uid="{AE380D6E-7373-4358-992A-5E58CE864723}"/>
     <hyperlink ref="A4" r:id="rId6" xr:uid="{48EDFAD1-D101-4B77-9288-82C0A0E67CAF}"/>
+    <hyperlink ref="A5" r:id="rId7" xr:uid="{4BF69A6C-8D40-4B4D-B53D-71DC1500C9BA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>